<commit_message>
technical and economic analysis
</commit_message>
<xml_diff>
--- a/Calculos/f chart method.xlsx
+++ b/Calculos/f chart method.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayte\OneDrive\Documentos\Documentos\Proyectos digitales\Heating-Systems-Peru\Calculos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886C32B-FBB9-49C9-9C95-692A8EBE50E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5E69DB-D5D7-4667-94F6-F34EABB5A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="2" xr2:uid="{871B7CCD-0AC1-4A84-B096-2B2F47B84CAF}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="21840" windowHeight="13020" xr2:uid="{871B7CCD-0AC1-4A84-B096-2B2F47B84CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada datos mensual" sheetId="10" r:id="rId1"/>
@@ -1136,7 +1136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1306,6 +1306,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1399,9 +1403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1572,40 +1573,40 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2442.833251012788</c:v>
+                  <c:v>1349.6822527338013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3053.4807824520049</c:v>
+                  <c:v>1746.8628279966576</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4321.107294828048</c:v>
+                  <c:v>2615.4170105352332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5039.0904273050328</c:v>
+                  <c:v>3146.6506993477828</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5623.3829286976552</c:v>
+                  <c:v>3658.793420344256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5956.2353149618402</c:v>
+                  <c:v>3972.0316100145728</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6364.4869175432332</c:v>
+                  <c:v>4330.8201153192531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5876.7030660714363</c:v>
+                  <c:v>3891.5165763427453</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4921.4948737742961</c:v>
+                  <c:v>3099.4184809776175</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3764.7901926131244</c:v>
+                  <c:v>2222.1546132829731</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2781.7112765357606</c:v>
+                  <c:v>1577.2522349701121</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2090.6072883796269</c:v>
+                  <c:v>1149.0859752167935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,40 +1876,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>510.57109359029658</c:v>
+                  <c:v>744.3184784012941</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>279.05428959091859</c:v>
+                  <c:v>558.44710017415093</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.5064446679837</c:v>
+                  <c:v>473.23249246803198</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-74.113621347463862</c:v>
+                  <c:v>330.54487324190694</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-144.28173581366985</c:v>
+                  <c:v>275.80447416802917</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-228.1107883683114</c:v>
+                  <c:v>196.16950565685787</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-271.41769531606275</c:v>
+                  <c:v>163.43924333668869</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-189.52756511770158</c:v>
+                  <c:v>234.96287679449469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-43.49333080049059</c:v>
+                  <c:v>346.11944219483041</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>213.10195687528397</c:v>
+                  <c:v>542.96218016787088</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>389.20660178789575</c:v>
+                  <c:v>646.75487418683679</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>570.43803049361861</c:v>
+                  <c:v>771.7625913659142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12005,15 +12006,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D77FBD-505A-47A8-B255-BE98960373ED}">
-  <dimension ref="A1:AA52"/>
+  <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="G27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
     <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
@@ -12025,61 +12026,62 @@
     <col min="10" max="10" width="19.21875" customWidth="1"/>
     <col min="11" max="11" width="21.77734375" customWidth="1"/>
     <col min="12" max="12" width="15.77734375" customWidth="1"/>
-    <col min="14" max="14" width="33.21875" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
       <c r="E2" s="22">
         <v>0.94</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="89"/>
+      <c r="H2" s="91"/>
       <c r="I2" s="22">
         <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
       <c r="E3" s="23">
         <v>1</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="91"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="23">
         <v>0.96</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="86"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="86"/>
+      <c r="G6" s="88"/>
       <c r="H6" s="21"/>
       <c r="I6" s="19"/>
       <c r="K6" s="9" t="s">
@@ -12091,20 +12093,20 @@
       <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="82"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="1">
         <v>-11.59</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="82"/>
+      <c r="G7" s="84"/>
       <c r="H7" s="6">
         <v>60</v>
       </c>
@@ -12122,10 +12124,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="1">
         <v>60</v>
       </c>
@@ -12147,10 +12149,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="1">
         <v>15</v>
       </c>
@@ -12163,10 +12165,10 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="1">
         <v>40</v>
       </c>
@@ -12179,10 +12181,10 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="18">
         <f>28*28</f>
         <v>784</v>
@@ -12202,17 +12204,17 @@
       <c r="F14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="98" t="s">
+      <c r="J14" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="98"/>
+      <c r="K14" s="100"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="89"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="10">
         <f>+L8</f>
         <v>1.9</v>
@@ -12220,20 +12222,20 @@
       <c r="D16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="96"/>
+      <c r="G16" s="98"/>
       <c r="H16" s="24">
-        <v>12</v>
-      </c>
-      <c r="J16" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="K16" s="89"/>
+      <c r="K16" s="91"/>
       <c r="L16" s="24">
         <f>75*H17</f>
-        <v>1709.9999999999998</v>
+        <v>854.99999999999989</v>
       </c>
       <c r="N16" t="s">
         <v>92</v>
@@ -12245,10 +12247,10 @@
       </c>
     </row>
     <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="94"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="27">
         <f>+D11/75</f>
         <v>10.453333333333333</v>
@@ -12256,21 +12258,21 @@
       <c r="D17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="90" t="s">
+      <c r="F17" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="91"/>
+      <c r="G17" s="93"/>
       <c r="H17" s="25">
         <f>+H16*C16</f>
-        <v>22.799999999999997</v>
+        <v>11.399999999999999</v>
       </c>
       <c r="I17" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="93" t="s">
+      <c r="J17" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="94"/>
+      <c r="K17" s="96"/>
       <c r="L17" s="26">
         <v>855</v>
       </c>
@@ -12283,22 +12285,22 @@
       </c>
     </row>
     <row r="18" spans="1:27" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="94"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="28">
         <f>+C17/C16</f>
         <v>5.5017543859649125</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="J18" s="90" t="s">
+      <c r="J18" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="91"/>
+      <c r="K18" s="93"/>
       <c r="L18" s="25">
         <f>+L17/H17</f>
-        <v>37.500000000000007</v>
+        <v>75.000000000000014</v>
       </c>
       <c r="N18" s="55" t="s">
         <v>107</v>
@@ -12309,10 +12311,10 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="91"/>
+      <c r="B19" s="93"/>
       <c r="C19" s="29">
         <f>ROUNDUP(C18*C16,0)</f>
         <v>11</v>
@@ -12356,21 +12358,21 @@
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="E23" s="97" t="s">
+      <c r="E23" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
       <c r="H23" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="E24" s="97" t="s">
+      <c r="E24" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
       <c r="H24" s="30">
         <v>0.15</v>
       </c>
@@ -12654,43 +12656,43 @@
       </c>
       <c r="H40" s="36">
         <f>+$P$20*$P$18*(100-E40)*3600*F40*B40*$H$17/(G40*10^6)</f>
-        <v>1.756269699272168</v>
+        <v>0.87813484963608401</v>
       </c>
       <c r="I40" s="36">
         <f>$P$16*$P$18*$P$17*D40*10^6*B40*$H$17/(G40*10^6)</f>
-        <v>0.70933582247546878</v>
+        <v>0.35466791123773439</v>
       </c>
       <c r="J40" s="52">
-        <f t="shared" ref="J40:J51" si="1">1.029*I40-0.065*H40-0.245*I40^2+0.0018*H40^2+0.0215*I40^3</f>
-        <v>0.50570107134832876</v>
+        <f>1.029*I40-0.065*H40-0.245*I40^2+0.0018*H40^2+0.0215*I40^3</f>
+        <v>0.27940333663967148</v>
       </c>
       <c r="K40" s="47">
-        <f t="shared" ref="K40:K51" si="2">+J40*G40</f>
-        <v>2442.833251012788</v>
+        <f>+J40*G40</f>
+        <v>1349.6822527338013</v>
       </c>
       <c r="L40" s="51">
         <f>+K40/(D40*$H$17*B40)</f>
-        <v>0.44310094811805978</v>
+        <v>0.48963267189565157</v>
       </c>
       <c r="M40" s="57">
         <f>+(G40-K40)*0.77*0.2777</f>
-        <v>510.57109359029658</v>
+        <v>744.3184784012941</v>
       </c>
       <c r="N40" s="58">
         <f>+G40*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>-215.00744171826602</v>
+        <v>222.75255828173385</v>
       </c>
       <c r="O40" s="2">
         <f>+(G40-K40)*$F$29</f>
-        <v>978.97922345435654</v>
+        <v>1427.171132748741</v>
       </c>
       <c r="P40" s="2">
         <f>+(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>9911.5999999999985</v>
+        <v>6263.5999999999995</v>
       </c>
       <c r="Q40" s="2">
         <f>+K40*J40*$C$29*0.277</f>
-        <v>249.18284511384445</v>
+        <v>76.066523700886606</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.3">
@@ -12718,43 +12720,43 @@
       </c>
       <c r="H41" s="36">
         <f>+$P$20*$P$18*(100-E41)*3600*F41*B41*$H$17/(G41*10^6)</f>
-        <v>1.5214513180499307</v>
+        <v>0.76072565902496536</v>
       </c>
       <c r="I41" s="36">
-        <f t="shared" ref="I41:I51" si="3">$P$16*$P$18*$P$17*D41*10^6*B41*$H$17/(G41*10^6)</f>
-        <v>0.98319288659830195</v>
+        <f t="shared" ref="I41:I51" si="1">$P$16*$P$18*$P$17*D41*10^6*B41*$H$17/(G41*10^6)</f>
+        <v>0.49159644329915098</v>
       </c>
       <c r="J41" s="52">
-        <f t="shared" si="1"/>
-        <v>0.7005781472474516</v>
+        <f t="shared" ref="J41:J51" si="2">1.029*I41-0.065*H41-0.245*I41^2+0.0018*H41^2+0.0215*I41^3</f>
+        <v>0.40079306559466721</v>
       </c>
       <c r="K41" s="47">
-        <f t="shared" si="2"/>
-        <v>3053.4807824520049</v>
+        <f t="shared" ref="K41:K51" si="3">+J41*G41</f>
+        <v>1746.8628279966576</v>
       </c>
       <c r="L41" s="51">
         <f t="shared" ref="L41:L51" si="4">+K41/(D41*$H$17*B41)</f>
-        <v>0.44287234034913747</v>
+        <v>0.50672480622756477</v>
       </c>
       <c r="M41" s="57">
         <f t="shared" ref="M41:M51" si="5">+(G41-K41)*0.77*0.2777</f>
-        <v>279.05428959091859</v>
+        <v>558.44710017415093</v>
       </c>
       <c r="N41" s="58">
-        <f t="shared" ref="N41:N51" si="6">+G41*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>-310.22971678944577</v>
+        <f>+G41*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
+        <v>127.5302832105541</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" ref="O41:O51" si="7">+(G41-K41)*$F$29</f>
-        <v>535.06427440747802</v>
+        <f>+(G41-K41)*$F$29</f>
+        <v>1070.7776357341702</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" ref="P41:P51" si="8">+(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>9911.5999999999985</v>
+        <f t="shared" ref="P41:P51" si="6">+(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
+        <v>6263.5999999999995</v>
       </c>
       <c r="Q41" s="2">
-        <f t="shared" ref="Q41:Q51" si="9">+K41*J41*$C$29*0.277</f>
-        <v>431.50141199263408</v>
+        <f t="shared" ref="Q41:Q51" si="7">+K41*J41*$C$29*0.277</f>
+        <v>141.2243049526318</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.3">
@@ -12782,43 +12784,43 @@
       </c>
       <c r="H42" s="36">
         <f>+$P$20*$P$18*(100-E42)*3600*F42*B42*$H$17/(G42*10^6)</f>
-        <v>1.8897510975967824</v>
+        <v>0.9448755487983912</v>
       </c>
       <c r="I42" s="36">
+        <f t="shared" si="1"/>
+        <v>0.69143904068012163</v>
+      </c>
+      <c r="J42" s="52">
+        <f t="shared" si="2"/>
+        <v>0.54165656325905442</v>
+      </c>
+      <c r="K42" s="47">
         <f t="shared" si="3"/>
-        <v>1.3828780813602433</v>
-      </c>
-      <c r="J42" s="52">
-        <f t="shared" si="1"/>
-        <v>0.89490743440228904</v>
-      </c>
-      <c r="K42" s="47">
-        <f t="shared" si="2"/>
-        <v>4321.107294828048</v>
+        <v>2615.4170105352332</v>
       </c>
       <c r="L42" s="51">
         <f t="shared" si="4"/>
-        <v>0.40221190529108664</v>
+        <v>0.48688995072961039</v>
       </c>
       <c r="M42" s="57">
-        <f t="shared" si="5"/>
-        <v>108.5064446679837</v>
+        <f>+(G42-K42)*0.77*0.2777</f>
+        <v>473.23249246803198</v>
       </c>
       <c r="N42" s="58">
+        <f t="shared" ref="N42:N51" si="8">+G42*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
+        <v>222.34203181942871</v>
+      </c>
+      <c r="O42" s="2">
+        <f t="shared" ref="O42:O51" si="9">+(G42-K42)*$F$29</f>
+        <v>907.38544309655424</v>
+      </c>
+      <c r="P42" s="2">
         <f t="shared" si="6"/>
-        <v>-215.41796818057117</v>
-      </c>
-      <c r="O42" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q42" s="2">
         <f t="shared" si="7"/>
-        <v>208.05242653650026</v>
-      </c>
-      <c r="P42" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q42" s="2">
-        <f t="shared" si="9"/>
-        <v>780.01617706929255</v>
+        <v>285.7560260239631</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
@@ -12846,43 +12848,43 @@
       </c>
       <c r="H43" s="36">
         <f>+$P$20*$P$18*(100-E43)*3600*F43*B43*$H$17/(G43*10^6)</f>
-        <v>1.0094049877849278</v>
+        <v>0.50470249389246391</v>
       </c>
       <c r="I43" s="36">
         <f>$P$16*$P$18*$P$17*D43*10^6*B43*$H$17/(G43*10^6)</f>
-        <v>1.6760437286271272</v>
+        <v>0.83802186431356362</v>
       </c>
       <c r="J43" s="52">
-        <f t="shared" si="1"/>
-        <v>1.0738632216554704</v>
+        <f t="shared" si="2"/>
+        <v>0.67057190303949721</v>
       </c>
       <c r="K43" s="47">
-        <f t="shared" si="2"/>
-        <v>5039.0904273050328</v>
+        <f t="shared" si="3"/>
+        <v>3146.6506993477828</v>
       </c>
       <c r="L43" s="51">
         <f>+K43/(D43*$H$17*B43)</f>
-        <v>0.39822114962107108</v>
+        <v>0.4973369210285733</v>
       </c>
       <c r="M43" s="57">
         <f t="shared" si="5"/>
-        <v>-74.113621347463862</v>
+        <v>330.54487324190694</v>
       </c>
       <c r="N43" s="58">
+        <f>+G43*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
+        <v>194.89635139595055</v>
+      </c>
+      <c r="O43" s="2">
+        <f t="shared" si="9"/>
+        <v>633.79334902740902</v>
+      </c>
+      <c r="P43" s="2">
         <f t="shared" si="6"/>
-        <v>-242.86364860404933</v>
-      </c>
-      <c r="O43" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q43" s="2">
         <f t="shared" si="7"/>
-        <v>-142.10693943506345</v>
-      </c>
-      <c r="P43" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q43" s="2">
-        <f t="shared" si="9"/>
-        <v>1091.5196644428565</v>
+        <v>425.62225859671065</v>
       </c>
       <c r="AA43" s="46"/>
     </row>
@@ -12911,43 +12913,43 @@
       </c>
       <c r="H44" s="36">
         <f t="shared" ref="H44:H51" si="10">+$P$20*$P$18*(100-E44)*3600*F44*B44*$H$17/(G44*10^6)</f>
-        <v>1.5448226584695113</v>
+        <v>0.77241132923475564</v>
       </c>
       <c r="I44" s="36">
+        <f t="shared" si="1"/>
+        <v>0.97204500189122978</v>
+      </c>
+      <c r="J44" s="52">
+        <f t="shared" si="2"/>
+        <v>0.73935480972942569</v>
+      </c>
+      <c r="K44" s="47">
         <f t="shared" si="3"/>
-        <v>1.9440900037824596</v>
-      </c>
-      <c r="J44" s="52">
-        <f t="shared" si="1"/>
-        <v>1.1363514518651778</v>
-      </c>
-      <c r="K44" s="47">
-        <f t="shared" si="2"/>
-        <v>5623.3829286976552</v>
+        <v>3658.793420344256</v>
       </c>
       <c r="L44" s="51">
-        <f t="shared" si="4"/>
-        <v>0.36329297707447655</v>
+        <f>+K44/(D44*$H$17*B44)</f>
+        <v>0.4727453104408133</v>
       </c>
       <c r="M44" s="57">
-        <f t="shared" si="5"/>
-        <v>-144.28173581366985</v>
+        <f>+(G44-K44)*0.77*0.2777</f>
+        <v>275.80447416802917</v>
       </c>
       <c r="N44" s="58">
         <f>+G44*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>-191.19690690455582</v>
+        <v>246.56309309544406</v>
       </c>
       <c r="O44" s="2">
+        <f t="shared" si="9"/>
+        <v>528.83301333725524</v>
+      </c>
+      <c r="P44" s="2">
+        <f t="shared" si="6"/>
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q44" s="2">
         <f t="shared" si="7"/>
-        <v>-276.64868508763846</v>
-      </c>
-      <c r="P44" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q44" s="2">
-        <f t="shared" si="9"/>
-        <v>1288.9639555767521</v>
+        <v>545.65889037016461</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.3">
@@ -12975,43 +12977,43 @@
       </c>
       <c r="H45" s="36">
         <f t="shared" si="10"/>
-        <v>1.2270759391622481</v>
+        <v>0.61353796958112405</v>
       </c>
       <c r="I45" s="36">
+        <f t="shared" si="1"/>
+        <v>1.07814942162339</v>
+      </c>
+      <c r="J45" s="52">
+        <f t="shared" si="2"/>
+        <v>0.81236866801122454</v>
+      </c>
+      <c r="K45" s="47">
         <f t="shared" si="3"/>
-        <v>2.15629884324678</v>
-      </c>
-      <c r="J45" s="52">
-        <f t="shared" si="1"/>
-        <v>1.2181823873146906</v>
-      </c>
-      <c r="K45" s="47">
-        <f t="shared" si="2"/>
-        <v>5956.2353149618402</v>
+        <v>3972.0316100145728</v>
       </c>
       <c r="L45" s="51">
         <f t="shared" si="4"/>
-        <v>0.35112686963319661</v>
+        <v>0.46831159333316513</v>
       </c>
       <c r="M45" s="57">
         <f t="shared" si="5"/>
-        <v>-228.1107883683114</v>
+        <v>196.16950565685787</v>
       </c>
       <c r="N45" s="58">
         <f>+G45*0.277*$C$29-$C$33*(($C$30+$C$32*$L$18)*$H$17+$C$31)</f>
-        <v>-203.13528128417749</v>
+        <v>234.62471871582238</v>
       </c>
       <c r="O45" s="2">
+        <f t="shared" si="9"/>
+        <v>376.13933245402501</v>
+      </c>
+      <c r="P45" s="2">
+        <f t="shared" si="6"/>
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q45" s="2">
         <f t="shared" si="7"/>
-        <v>-437.38418657435454</v>
-      </c>
-      <c r="P45" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q45" s="2">
-        <f t="shared" si="9"/>
-        <v>1463.5737346047081</v>
+        <v>650.87307250928086</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.3">
@@ -13039,43 +13041,43 @@
       </c>
       <c r="H46" s="36">
         <f t="shared" si="10"/>
-        <v>1.3357165795545218</v>
+        <v>0.66785828977726092</v>
       </c>
       <c r="I46" s="36">
-        <f t="shared" si="3"/>
-        <v>2.3020258275867902</v>
+        <f>$P$16*$P$18*$P$17*D46*10^6*B46*$H$17/(G46*10^6)</f>
+        <v>1.1510129137933951</v>
       </c>
       <c r="J46" s="52">
-        <f t="shared" si="1"/>
-        <v>1.2491226670621487</v>
+        <f t="shared" si="2"/>
+        <v>0.84998612505628424</v>
       </c>
       <c r="K46" s="47">
-        <f t="shared" si="2"/>
-        <v>6364.4869175432332</v>
+        <f>+J46*G46</f>
+        <v>4330.8201153192531</v>
       </c>
       <c r="L46" s="51">
         <f t="shared" si="4"/>
-        <v>0.33725282475551749</v>
+        <v>0.45897849624718395</v>
       </c>
       <c r="M46" s="57">
         <f t="shared" si="5"/>
-        <v>-271.41769531606275</v>
+        <v>163.43924333668869</v>
       </c>
       <c r="N46" s="58">
+        <f t="shared" si="8"/>
+        <v>276.12099838142865</v>
+      </c>
+      <c r="O46" s="2">
+        <f t="shared" si="9"/>
+        <v>313.38167305670589</v>
+      </c>
+      <c r="P46" s="2">
         <f t="shared" si="6"/>
-        <v>-161.63900161857123</v>
-      </c>
-      <c r="O46" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q46" s="2">
         <f t="shared" si="7"/>
-        <v>-520.42171585512597</v>
-      </c>
-      <c r="P46" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q46" s="2">
-        <f t="shared" si="9"/>
-        <v>1603.6106471522733</v>
+        <v>742.52729950292849</v>
       </c>
       <c r="X46" s="8"/>
       <c r="Y46" s="8"/>
@@ -13105,43 +13107,43 @@
       </c>
       <c r="H47" s="36">
         <f t="shared" si="10"/>
-        <v>1.534242358902564</v>
+        <v>0.767121179451282</v>
       </c>
       <c r="I47" s="36">
+        <f t="shared" si="1"/>
+        <v>1.0387428985661729</v>
+      </c>
+      <c r="J47" s="52">
+        <f t="shared" si="2"/>
+        <v>0.77980803504891893</v>
+      </c>
+      <c r="K47" s="47">
         <f t="shared" si="3"/>
-        <v>2.0774857971323457</v>
-      </c>
-      <c r="J47" s="52">
-        <f t="shared" si="1"/>
-        <v>1.1776129384564911</v>
-      </c>
-      <c r="K47" s="47">
-        <f t="shared" si="2"/>
-        <v>5876.7030660714363</v>
+        <v>3891.5165763427453</v>
       </c>
       <c r="L47" s="51">
         <f t="shared" si="4"/>
-        <v>0.35231018927941149</v>
+        <v>0.46659527499721187</v>
       </c>
       <c r="M47" s="57">
         <f t="shared" si="5"/>
-        <v>-189.52756511770158</v>
+        <v>234.96287679449469</v>
       </c>
       <c r="N47" s="58">
+        <f t="shared" si="8"/>
+        <v>254.97888557270358</v>
+      </c>
+      <c r="O47" s="2">
+        <f t="shared" si="9"/>
+        <v>450.5225179266742</v>
+      </c>
+      <c r="P47" s="2">
         <f t="shared" si="6"/>
-        <v>-182.7811144272963</v>
-      </c>
-      <c r="O47" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q47" s="2">
         <f t="shared" si="7"/>
-        <v>-363.40394286208902</v>
-      </c>
-      <c r="P47" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q47" s="2">
-        <f t="shared" si="9"/>
-        <v>1395.9400253667077</v>
+        <v>612.12065482191554</v>
       </c>
       <c r="X47" s="8"/>
       <c r="Y47" s="8"/>
@@ -13171,43 +13173,43 @@
       </c>
       <c r="H48" s="36">
         <f t="shared" si="10"/>
-        <v>1.6349670018625722</v>
+        <v>0.81748350093128608</v>
       </c>
       <c r="I48" s="36">
+        <f t="shared" si="1"/>
+        <v>0.84698984750616491</v>
+      </c>
+      <c r="J48" s="52">
+        <f t="shared" si="2"/>
+        <v>0.65692194359630129</v>
+      </c>
+      <c r="K48" s="47">
         <f t="shared" si="3"/>
-        <v>1.6939796950123298</v>
-      </c>
-      <c r="J48" s="52">
-        <f t="shared" si="1"/>
-        <v>1.0431111505985731</v>
-      </c>
-      <c r="K48" s="47">
-        <f t="shared" si="2"/>
-        <v>4921.4948737742961</v>
+        <v>3099.4184809776175</v>
       </c>
       <c r="L48" s="51">
         <f t="shared" si="4"/>
-        <v>0.38272169915502491</v>
+        <v>0.48205463496603485</v>
       </c>
       <c r="M48" s="57">
         <f t="shared" si="5"/>
-        <v>-43.49333080049059</v>
+        <v>346.11944219483041</v>
       </c>
       <c r="N48" s="58">
+        <f t="shared" si="8"/>
+        <v>200.06103914753362</v>
+      </c>
+      <c r="O48" s="2">
+        <f t="shared" si="9"/>
+        <v>663.65633894317637</v>
+      </c>
+      <c r="P48" s="2">
         <f t="shared" si="6"/>
-        <v>-237.69896085246626</v>
-      </c>
-      <c r="O48" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q48" s="2">
         <f t="shared" si="7"/>
-        <v>-83.394982103461828</v>
-      </c>
-      <c r="P48" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q48" s="2">
-        <f t="shared" si="9"/>
-        <v>1035.5189923907553</v>
+        <v>410.69974299628706</v>
       </c>
       <c r="X48" s="8"/>
       <c r="Y48" s="8"/>
@@ -13238,43 +13240,43 @@
       </c>
       <c r="H49" s="36">
         <f t="shared" si="10"/>
-        <v>2.0069653206179834</v>
+        <v>1.0034826603089917</v>
       </c>
       <c r="I49" s="36">
+        <f t="shared" si="1"/>
+        <v>0.59509073856805028</v>
+      </c>
+      <c r="J49" s="52">
+        <f t="shared" si="2"/>
+        <v>0.46670291173743006</v>
+      </c>
+      <c r="K49" s="47">
         <f t="shared" si="3"/>
-        <v>1.1901814771361006</v>
-      </c>
-      <c r="J49" s="52">
-        <f t="shared" si="1"/>
-        <v>0.7906914012509898</v>
-      </c>
-      <c r="K49" s="47">
-        <f t="shared" si="2"/>
-        <v>3764.7901926131244</v>
+        <v>2222.1546132829731</v>
       </c>
       <c r="L49" s="51">
         <f t="shared" si="4"/>
-        <v>0.41290916946485806</v>
+        <v>0.48743646729291396</v>
       </c>
       <c r="M49" s="57">
         <f t="shared" si="5"/>
-        <v>213.10195687528397</v>
+        <v>542.96218016787088</v>
       </c>
       <c r="N49" s="58">
+        <f t="shared" si="8"/>
+        <v>208.79465856335253</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="9"/>
+        <v>1041.0865405011812</v>
+      </c>
+      <c r="P49" s="2">
         <f t="shared" si="6"/>
-        <v>-228.96534143664735</v>
-      </c>
-      <c r="O49" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q49" s="2">
         <f t="shared" si="7"/>
-        <v>408.60595297581909</v>
-      </c>
-      <c r="P49" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q49" s="2">
-        <f t="shared" si="9"/>
-        <v>600.45192023288769</v>
+        <v>209.19207469890335</v>
       </c>
       <c r="X49" s="8"/>
       <c r="Y49" s="8"/>
@@ -13305,43 +13307,43 @@
       </c>
       <c r="H50" s="36">
         <f t="shared" si="10"/>
-        <v>2.1320752688248641</v>
+        <v>1.066037634412432</v>
       </c>
       <c r="I50" s="36">
+        <f t="shared" si="1"/>
+        <v>0.44342684150073908</v>
+      </c>
+      <c r="J50" s="52">
+        <f t="shared" si="2"/>
+        <v>0.34274023656743219</v>
+      </c>
+      <c r="K50" s="47">
         <f t="shared" si="3"/>
-        <v>0.88685368300147815</v>
-      </c>
-      <c r="J50" s="52">
-        <f t="shared" si="1"/>
-        <v>0.6044717261093161</v>
-      </c>
-      <c r="K50" s="47">
-        <f t="shared" si="2"/>
-        <v>2781.7112765357606</v>
+        <v>1577.2522349701121</v>
       </c>
       <c r="L50" s="51">
         <f t="shared" si="4"/>
-        <v>0.42362805746463222</v>
+        <v>0.48040090002744651</v>
       </c>
       <c r="M50" s="57">
         <f t="shared" si="5"/>
-        <v>389.20660178789575</v>
+        <v>646.75487418683679</v>
       </c>
       <c r="N50" s="58">
+        <f t="shared" si="8"/>
+        <v>176.62130242880937</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="9"/>
+        <v>1240.1007272942541</v>
+      </c>
+      <c r="P50" s="2">
         <f t="shared" si="6"/>
-        <v>-261.13869757119051</v>
-      </c>
-      <c r="O50" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q50" s="2">
         <f t="shared" si="7"/>
-        <v>746.27252025233827</v>
-      </c>
-      <c r="P50" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q50" s="2">
-        <f t="shared" si="9"/>
-        <v>339.17082397204734</v>
+        <v>109.04272279603896</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.3">
@@ -13369,43 +13371,43 @@
       </c>
       <c r="H51" s="36">
         <f t="shared" si="10"/>
-        <v>2.2286709426980806</v>
+        <v>1.1143354713490403</v>
       </c>
       <c r="I51" s="36">
+        <f t="shared" si="1"/>
+        <v>0.32774069662826077</v>
+      </c>
+      <c r="J51" s="52">
+        <f t="shared" si="2"/>
+        <v>0.24148897277466005</v>
+      </c>
+      <c r="K51" s="47">
         <f t="shared" si="3"/>
-        <v>0.65548139325652155</v>
-      </c>
-      <c r="J51" s="52">
-        <f t="shared" si="1"/>
-        <v>0.43935668647488629</v>
-      </c>
-      <c r="K51" s="47">
-        <f t="shared" si="2"/>
-        <v>2090.6072883796269</v>
+        <v>1149.0859752167935</v>
       </c>
       <c r="L51" s="51">
         <f t="shared" si="4"/>
-        <v>0.41659837402050648</v>
+        <v>0.45796008800497134</v>
       </c>
       <c r="M51" s="57">
         <f t="shared" si="5"/>
-        <v>570.43803049361861</v>
+        <v>771.7625913659142</v>
       </c>
       <c r="N51" s="58">
+        <f t="shared" si="8"/>
+        <v>208.17886886989436</v>
+      </c>
+      <c r="O51" s="2">
+        <f t="shared" si="9"/>
+        <v>1479.7930236779146</v>
+      </c>
+      <c r="P51" s="2">
         <f t="shared" si="6"/>
-        <v>-229.58113113010552</v>
-      </c>
-      <c r="O51" s="2">
+        <v>6263.5999999999995</v>
+      </c>
+      <c r="Q51" s="2">
         <f t="shared" si="7"/>
-        <v>1093.7692852811529</v>
-      </c>
-      <c r="P51" s="2">
-        <f t="shared" si="8"/>
-        <v>9911.5999999999985</v>
-      </c>
-      <c r="Q51" s="2">
-        <f t="shared" si="9"/>
-        <v>185.27641723726336</v>
+        <v>55.973217467155024</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.3">
@@ -13420,33 +13422,36 @@
       <c r="H52" s="34"/>
       <c r="J52" s="53">
         <f>+K52/G52</f>
-        <v>0.90887060632981842</v>
+        <v>0.56999691881902259</v>
       </c>
       <c r="K52" s="50">
         <f>+SUM(K40:K51)</f>
-        <v>52235.923614174848</v>
+        <v>32759.685817081798</v>
       </c>
       <c r="L52" s="54">
         <f>+K52/(AVERAGE(D40:D51)*365*H17)</f>
-        <v>0.38099225165958533</v>
+        <v>0.47787750649530608</v>
       </c>
       <c r="M52" s="8">
         <f>+SUM(M40:M51)</f>
-        <v>1119.9336802422972</v>
+        <v>5284.5181321569062</v>
       </c>
       <c r="N52" s="5">
         <f>+SUM(N40:N51)</f>
-        <v>-2679.6552105173428</v>
+        <v>2573.4647894826562</v>
       </c>
       <c r="O52" s="31">
         <f>+SUM(O40:O51)</f>
-        <v>2147.3832309899117</v>
+        <v>10132.64072779806</v>
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" s="2">
         <f>+SUM(Q40:Q51)</f>
-        <v>10464.726615152022</v>
-      </c>
+        <v>4264.7567884368664</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="L53" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -13524,44 +13529,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="101"/>
-      <c r="C1" s="102" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="104" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="104"/>
+      <c r="E1" s="104" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="101"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="79" t="s">
         <v>153</v>
       </c>
       <c r="D2" s="79" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="105" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="103"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="79" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="99">
+      <c r="A3" s="101">
         <v>1</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="101">
+      <c r="C3" s="103">
         <v>7.38</v>
       </c>
-      <c r="D3" s="101">
+      <c r="D3" s="103">
         <v>4.46</v>
       </c>
       <c r="E3" s="2">
@@ -13570,32 +13575,32 @@
       <c r="F3" s="2">
         <v>1872.23</v>
       </c>
-      <c r="G3" s="101">
+      <c r="G3" s="103">
         <v>1589.45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101">
+      <c r="A4" s="101"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103">
         <v>2657.66</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="99">
+      <c r="A5" s="101">
         <v>2</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="101">
+      <c r="C5" s="103">
         <v>6.68</v>
       </c>
-      <c r="D5" s="101">
+      <c r="D5" s="103">
         <v>0</v>
       </c>
       <c r="E5" s="2">
@@ -13604,32 +13609,32 @@
       <c r="F5" s="2">
         <v>1872.23</v>
       </c>
-      <c r="G5" s="101">
+      <c r="G5" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="99"/>
-      <c r="B6" s="100"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101">
+      <c r="A6" s="101"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103">
         <v>4349.78</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="99">
+      <c r="A7" s="101">
         <v>3</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="101">
+      <c r="C7" s="103">
         <v>21.56</v>
       </c>
-      <c r="D7" s="101">
+      <c r="D7" s="103">
         <v>9.42</v>
       </c>
       <c r="E7" s="2">
@@ -13638,32 +13643,32 @@
       <c r="F7" s="2">
         <v>1877.62</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="103">
         <v>8565.36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101">
+      <c r="A8" s="101"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103">
         <v>23061.599999999999</v>
       </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="99">
+      <c r="A9" s="101">
         <v>4</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="101">
+      <c r="C9" s="103">
         <v>6.68</v>
       </c>
-      <c r="D9" s="101">
+      <c r="D9" s="103">
         <v>0.8</v>
       </c>
       <c r="E9" s="2">
@@ -13672,32 +13677,32 @@
       <c r="F9" s="2">
         <v>1872.33</v>
       </c>
-      <c r="G9" s="101">
+      <c r="G9" s="103">
         <v>2.77</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="99"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101">
+      <c r="A10" s="101"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103">
         <v>3930.88</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="99">
+      <c r="A11" s="101">
         <v>5</v>
       </c>
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="102" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="101">
+      <c r="C11" s="103">
         <v>6.68</v>
       </c>
-      <c r="D11" s="101">
+      <c r="D11" s="103">
         <v>0</v>
       </c>
       <c r="E11" s="2">
@@ -13706,32 +13711,32 @@
       <c r="F11" s="2">
         <v>1872.23</v>
       </c>
-      <c r="G11" s="101">
+      <c r="G11" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101">
+      <c r="A12" s="101"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103">
         <v>4349.78</v>
       </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="99">
+      <c r="A13" s="101">
         <v>6</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="C13" s="101">
+      <c r="C13" s="103">
         <v>21.56</v>
       </c>
-      <c r="D13" s="101">
+      <c r="D13" s="103">
         <v>9.42</v>
       </c>
       <c r="E13" s="2">
@@ -13740,20 +13745,20 @@
       <c r="F13" s="2">
         <v>1877.62</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="103">
         <v>8565.36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101">
+      <c r="A14" s="101"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103">
         <v>23061.599999999999</v>
       </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -13807,7 +13812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6AE83B0-A4A9-44CA-9133-56EE86115956}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -13817,7 +13822,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112">
+      <c r="A1" s="81">
         <v>45000</v>
       </c>
     </row>
@@ -13894,10 +13899,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="1">
         <v>-11.59</v>
       </c>
@@ -13906,10 +13911,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="1">
         <v>60</v>
       </c>
@@ -13918,10 +13923,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="82"/>
+      <c r="B3" s="84"/>
       <c r="C3" s="1">
         <v>15</v>
       </c>
@@ -13930,10 +13935,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="82"/>
+      <c r="B4" s="84"/>
       <c r="C4" s="1">
         <v>40</v>
       </c>
@@ -13942,10 +13947,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="84"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="18">
         <v>2800</v>
       </c>
@@ -14229,36 +14234,36 @@
     </row>
     <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="106"/>
-      <c r="D26" s="104" t="s">
+      <c r="B26" s="107"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="105"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="107" t="s">
+      <c r="E26" s="107"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="108"/>
-      <c r="I26" s="109"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="111"/>
       <c r="K26" s="9"/>
       <c r="L26" s="24">
         <v>0.77</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="105"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="109"/>
+      <c r="A27" s="107"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="111"/>
       <c r="K27" s="12"/>
       <c r="L27" s="26">
         <v>0.96</v>
@@ -14272,17 +14277,17 @@
         <v>1.9</v>
       </c>
       <c r="C28" s="32"/>
-      <c r="D28" s="111" t="s">
+      <c r="D28" s="113" t="s">
         <v>77</v>
       </c>
       <c r="E28">
         <v>18</v>
       </c>
       <c r="F28" s="32"/>
-      <c r="G28" s="111" t="s">
+      <c r="G28" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="108">
+      <c r="H28" s="110">
         <v>2565</v>
       </c>
       <c r="I28" s="32"/>
@@ -14299,10 +14304,10 @@
         <v>37.33</v>
       </c>
       <c r="C29" s="32"/>
-      <c r="D29" s="111"/>
+      <c r="D29" s="113"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="108"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="110"/>
       <c r="I29" s="32"/>
       <c r="K29" s="12"/>
       <c r="L29" s="13">
@@ -14317,17 +14322,17 @@
         <v>20</v>
       </c>
       <c r="C30" s="32"/>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="113" t="s">
         <v>78</v>
       </c>
       <c r="E30">
         <v>34.200000000000003</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="111" t="s">
+      <c r="G30" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="108">
+      <c r="H30" s="110">
         <v>2565</v>
       </c>
       <c r="I30" s="32"/>
@@ -14347,10 +14352,10 @@
         <v>38</v>
       </c>
       <c r="C31" s="32"/>
-      <c r="D31" s="111"/>
+      <c r="D31" s="113"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="111"/>
-      <c r="H31" s="108"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="110"/>
       <c r="I31" s="32"/>
       <c r="K31" s="12"/>
       <c r="L31" s="26">
@@ -14376,25 +14381,25 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="110" t="s">
+      <c r="B34" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
       <c r="G34" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="110" t="s">
+      <c r="B36" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="110"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
       <c r="G36" t="s">
         <v>82</v>
       </c>
@@ -14430,7 +14435,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A10" activeCellId="1" sqref="I10:I22 A10:A22"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14939,7 +14944,7 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>